<commit_message>
[PGE] Add 2020-06-20 data (correct martinique and guyane)
</commit_message>
<xml_diff>
--- a/published-data/pge-departemental-naf-latest.xlsx
+++ b/published-data/pge-departemental-naf-latest.xlsx
@@ -1126,120 +1126,120 @@
     <t>169.00</t>
   </si>
   <si>
+    <t>163.00</t>
+  </si>
+  <si>
+    <t>397.00</t>
+  </si>
+  <si>
+    <t>566.00</t>
+  </si>
+  <si>
+    <t>340.00</t>
+  </si>
+  <si>
+    <t>967.00</t>
+  </si>
+  <si>
+    <t>1807.00</t>
+  </si>
+  <si>
+    <t>3206.00</t>
+  </si>
+  <si>
+    <t>369.00</t>
+  </si>
+  <si>
+    <t>2169.00</t>
+  </si>
+  <si>
+    <t>1344.00</t>
+  </si>
+  <si>
+    <t>303.00</t>
+  </si>
+  <si>
+    <t>1218.00</t>
+  </si>
+  <si>
+    <t>239.00</t>
+  </si>
+  <si>
+    <t>997.00</t>
+  </si>
+  <si>
+    <t>647.00</t>
+  </si>
+  <si>
+    <t>979.00</t>
+  </si>
+  <si>
+    <t>470.00</t>
+  </si>
+  <si>
+    <t>54.00</t>
+  </si>
+  <si>
+    <t>98.00</t>
+  </si>
+  <si>
+    <t>311.00</t>
+  </si>
+  <si>
+    <t>1116.00</t>
+  </si>
+  <si>
+    <t>1751.00</t>
+  </si>
+  <si>
+    <t>1131.00</t>
+  </si>
+  <si>
+    <t>187.00</t>
+  </si>
+  <si>
+    <t>611.00</t>
+  </si>
+  <si>
+    <t>659.00</t>
+  </si>
+  <si>
+    <t>516.00</t>
+  </si>
+  <si>
+    <t>175.00</t>
+  </si>
+  <si>
+    <t>125.00</t>
+  </si>
+  <si>
+    <t>488.00</t>
+  </si>
+  <si>
+    <t>774.00</t>
+  </si>
+  <si>
+    <t>1493.00</t>
+  </si>
+  <si>
+    <t>535.00</t>
+  </si>
+  <si>
+    <t>362.00</t>
+  </si>
+  <si>
+    <t>209.00</t>
+  </si>
+  <si>
     <t>230.00</t>
   </si>
   <si>
     <t>118.00</t>
   </si>
   <si>
-    <t>239.00</t>
-  </si>
-  <si>
     <t>219.00</t>
   </si>
   <si>
-    <t>397.00</t>
-  </si>
-  <si>
-    <t>566.00</t>
-  </si>
-  <si>
-    <t>340.00</t>
-  </si>
-  <si>
-    <t>967.00</t>
-  </si>
-  <si>
-    <t>1807.00</t>
-  </si>
-  <si>
-    <t>3206.00</t>
-  </si>
-  <si>
-    <t>369.00</t>
-  </si>
-  <si>
-    <t>2169.00</t>
-  </si>
-  <si>
-    <t>1344.00</t>
-  </si>
-  <si>
-    <t>303.00</t>
-  </si>
-  <si>
-    <t>1218.00</t>
-  </si>
-  <si>
-    <t>997.00</t>
-  </si>
-  <si>
-    <t>647.00</t>
-  </si>
-  <si>
-    <t>979.00</t>
-  </si>
-  <si>
-    <t>470.00</t>
-  </si>
-  <si>
-    <t>54.00</t>
-  </si>
-  <si>
-    <t>98.00</t>
-  </si>
-  <si>
-    <t>311.00</t>
-  </si>
-  <si>
-    <t>1116.00</t>
-  </si>
-  <si>
-    <t>1751.00</t>
-  </si>
-  <si>
-    <t>1131.00</t>
-  </si>
-  <si>
-    <t>187.00</t>
-  </si>
-  <si>
-    <t>611.00</t>
-  </si>
-  <si>
-    <t>659.00</t>
-  </si>
-  <si>
-    <t>516.00</t>
-  </si>
-  <si>
-    <t>175.00</t>
-  </si>
-  <si>
-    <t>125.00</t>
-  </si>
-  <si>
-    <t>488.00</t>
-  </si>
-  <si>
-    <t>774.00</t>
-  </si>
-  <si>
-    <t>1493.00</t>
-  </si>
-  <si>
-    <t>535.00</t>
-  </si>
-  <si>
-    <t>362.00</t>
-  </si>
-  <si>
-    <t>209.00</t>
-  </si>
-  <si>
-    <t>163.00</t>
-  </si>
-  <si>
     <t>1164.00</t>
   </si>
   <si>
@@ -4171,6 +4171,369 @@
     <t>2961915.00</t>
   </si>
   <si>
+    <t>1230800.00</t>
+  </si>
+  <si>
+    <t>849000.00</t>
+  </si>
+  <si>
+    <t>13498461.00</t>
+  </si>
+  <si>
+    <t>11612170.00</t>
+  </si>
+  <si>
+    <t>43888731.00</t>
+  </si>
+  <si>
+    <t>20987900.00</t>
+  </si>
+  <si>
+    <t>5328500.00</t>
+  </si>
+  <si>
+    <t>2031700.00</t>
+  </si>
+  <si>
+    <t>1922000.00</t>
+  </si>
+  <si>
+    <t>2641349.00</t>
+  </si>
+  <si>
+    <t>6120100.00</t>
+  </si>
+  <si>
+    <t>7327053.00</t>
+  </si>
+  <si>
+    <t>1539200.00</t>
+  </si>
+  <si>
+    <t>4152549.00</t>
+  </si>
+  <si>
+    <t>968000.00</t>
+  </si>
+  <si>
+    <t>1328600.00</t>
+  </si>
+  <si>
+    <t>7495201.00</t>
+  </si>
+  <si>
+    <t>52167283.00</t>
+  </si>
+  <si>
+    <t>708000.00</t>
+  </si>
+  <si>
+    <t>191625682.00</t>
+  </si>
+  <si>
+    <t>104968337.00</t>
+  </si>
+  <si>
+    <t>13539850.00</t>
+  </si>
+  <si>
+    <t>26767132.00</t>
+  </si>
+  <si>
+    <t>5801733.00</t>
+  </si>
+  <si>
+    <t>6201041.00</t>
+  </si>
+  <si>
+    <t>2948915.00</t>
+  </si>
+  <si>
+    <t>17078365.00</t>
+  </si>
+  <si>
+    <t>6242240.00</t>
+  </si>
+  <si>
+    <t>1848857.00</t>
+  </si>
+  <si>
+    <t>10445920.00</t>
+  </si>
+  <si>
+    <t>2959555.00</t>
+  </si>
+  <si>
+    <t>4511994.00</t>
+  </si>
+  <si>
+    <t>454000.00</t>
+  </si>
+  <si>
+    <t>11916979.00</t>
+  </si>
+  <si>
+    <t>372778451.00</t>
+  </si>
+  <si>
+    <t>966877.00</t>
+  </si>
+  <si>
+    <t>20205950.00</t>
+  </si>
+  <si>
+    <t>285413924.00</t>
+  </si>
+  <si>
+    <t>1612533045.00</t>
+  </si>
+  <si>
+    <t>139443583.00</t>
+  </si>
+  <si>
+    <t>147781820.00</t>
+  </si>
+  <si>
+    <t>84230036.00</t>
+  </si>
+  <si>
+    <t>304186987.00</t>
+  </si>
+  <si>
+    <t>31693829.00</t>
+  </si>
+  <si>
+    <t>234843798.00</t>
+  </si>
+  <si>
+    <t>87070119.00</t>
+  </si>
+  <si>
+    <t>22413089.00</t>
+  </si>
+  <si>
+    <t>76743216.00</t>
+  </si>
+  <si>
+    <t>21653619.00</t>
+  </si>
+  <si>
+    <t>35393271.00</t>
+  </si>
+  <si>
+    <t>2411447.00</t>
+  </si>
+  <si>
+    <t>5842500.00</t>
+  </si>
+  <si>
+    <t>103655077.00</t>
+  </si>
+  <si>
+    <t>2056000.00</t>
+  </si>
+  <si>
+    <t>88499437.00</t>
+  </si>
+  <si>
+    <t>159068243.00</t>
+  </si>
+  <si>
+    <t>27785208.00</t>
+  </si>
+  <si>
+    <t>31945979.00</t>
+  </si>
+  <si>
+    <t>6180541.00</t>
+  </si>
+  <si>
+    <t>55321896.00</t>
+  </si>
+  <si>
+    <t>7740251.00</t>
+  </si>
+  <si>
+    <t>29609970.00</t>
+  </si>
+  <si>
+    <t>29179890.00</t>
+  </si>
+  <si>
+    <t>4890364.00</t>
+  </si>
+  <si>
+    <t>33690661.00</t>
+  </si>
+  <si>
+    <t>9679859.00</t>
+  </si>
+  <si>
+    <t>7494508.00</t>
+  </si>
+  <si>
+    <t>700000.00</t>
+  </si>
+  <si>
+    <t>5742520.00</t>
+  </si>
+  <si>
+    <t>223044993.00</t>
+  </si>
+  <si>
+    <t>7564000.00</t>
+  </si>
+  <si>
+    <t>139756795.00</t>
+  </si>
+  <si>
+    <t>284386452.00</t>
+  </si>
+  <si>
+    <t>58361793.00</t>
+  </si>
+  <si>
+    <t>88760577.00</t>
+  </si>
+  <si>
+    <t>5890854.00</t>
+  </si>
+  <si>
+    <t>47245789.00</t>
+  </si>
+  <si>
+    <t>9613708.00</t>
+  </si>
+  <si>
+    <t>47347226.00</t>
+  </si>
+  <si>
+    <t>21662068.00</t>
+  </si>
+  <si>
+    <t>6534259.00</t>
+  </si>
+  <si>
+    <t>38796984.00</t>
+  </si>
+  <si>
+    <t>15126914.00</t>
+  </si>
+  <si>
+    <t>12751832.00</t>
+  </si>
+  <si>
+    <t>2288000.00</t>
+  </si>
+  <si>
+    <t>9328825.00</t>
+  </si>
+  <si>
+    <t>92762230.00</t>
+  </si>
+  <si>
+    <t>720898.00</t>
+  </si>
+  <si>
+    <t>43688264.00</t>
+  </si>
+  <si>
+    <t>102603673.00</t>
+  </si>
+  <si>
+    <t>8131180.00</t>
+  </si>
+  <si>
+    <t>37077612.00</t>
+  </si>
+  <si>
+    <t>3183160.00</t>
+  </si>
+  <si>
+    <t>65432830.00</t>
+  </si>
+  <si>
+    <t>8022840.00</t>
+  </si>
+  <si>
+    <t>18443424.00</t>
+  </si>
+  <si>
+    <t>6106728.00</t>
+  </si>
+  <si>
+    <t>10127359.00</t>
+  </si>
+  <si>
+    <t>16115000.00</t>
+  </si>
+  <si>
+    <t>8818400.00</t>
+  </si>
+  <si>
+    <t>5263308.00</t>
+  </si>
+  <si>
+    <t>697000.00</t>
+  </si>
+  <si>
+    <t>14035102.00</t>
+  </si>
+  <si>
+    <t>2350000.00</t>
+  </si>
+  <si>
+    <t>76568063.00</t>
+  </si>
+  <si>
+    <t>793343.00</t>
+  </si>
+  <si>
+    <t>4517000.00</t>
+  </si>
+  <si>
+    <t>93471025.00</t>
+  </si>
+  <si>
+    <t>330513760.00</t>
+  </si>
+  <si>
+    <t>94085244.00</t>
+  </si>
+  <si>
+    <t>46244692.00</t>
+  </si>
+  <si>
+    <t>10822326.00</t>
+  </si>
+  <si>
+    <t>35235230.00</t>
+  </si>
+  <si>
+    <t>5089773.00</t>
+  </si>
+  <si>
+    <t>96547076.00</t>
+  </si>
+  <si>
+    <t>29748444.00</t>
+  </si>
+  <si>
+    <t>8913852.00</t>
+  </si>
+  <si>
+    <t>28820755.00</t>
+  </si>
+  <si>
+    <t>7455107.00</t>
+  </si>
+  <si>
+    <t>10103771.00</t>
+  </si>
+  <si>
+    <t>287500.00</t>
+  </si>
+  <si>
     <t>9638506.00</t>
   </si>
   <si>
@@ -4223,369 +4586,6 @@
   </si>
   <si>
     <t>429962.00</t>
-  </si>
-  <si>
-    <t>7495201.00</t>
-  </si>
-  <si>
-    <t>52167283.00</t>
-  </si>
-  <si>
-    <t>708000.00</t>
-  </si>
-  <si>
-    <t>191625682.00</t>
-  </si>
-  <si>
-    <t>104968337.00</t>
-  </si>
-  <si>
-    <t>13539850.00</t>
-  </si>
-  <si>
-    <t>26767132.00</t>
-  </si>
-  <si>
-    <t>5801733.00</t>
-  </si>
-  <si>
-    <t>6201041.00</t>
-  </si>
-  <si>
-    <t>2948915.00</t>
-  </si>
-  <si>
-    <t>17078365.00</t>
-  </si>
-  <si>
-    <t>6242240.00</t>
-  </si>
-  <si>
-    <t>1848857.00</t>
-  </si>
-  <si>
-    <t>10445920.00</t>
-  </si>
-  <si>
-    <t>2959555.00</t>
-  </si>
-  <si>
-    <t>4511994.00</t>
-  </si>
-  <si>
-    <t>454000.00</t>
-  </si>
-  <si>
-    <t>11916979.00</t>
-  </si>
-  <si>
-    <t>372778451.00</t>
-  </si>
-  <si>
-    <t>966877.00</t>
-  </si>
-  <si>
-    <t>20205950.00</t>
-  </si>
-  <si>
-    <t>285413924.00</t>
-  </si>
-  <si>
-    <t>1612533045.00</t>
-  </si>
-  <si>
-    <t>139443583.00</t>
-  </si>
-  <si>
-    <t>147781820.00</t>
-  </si>
-  <si>
-    <t>84230036.00</t>
-  </si>
-  <si>
-    <t>304186987.00</t>
-  </si>
-  <si>
-    <t>31693829.00</t>
-  </si>
-  <si>
-    <t>234843798.00</t>
-  </si>
-  <si>
-    <t>87070119.00</t>
-  </si>
-  <si>
-    <t>22413089.00</t>
-  </si>
-  <si>
-    <t>76743216.00</t>
-  </si>
-  <si>
-    <t>21653619.00</t>
-  </si>
-  <si>
-    <t>35393271.00</t>
-  </si>
-  <si>
-    <t>2411447.00</t>
-  </si>
-  <si>
-    <t>5842500.00</t>
-  </si>
-  <si>
-    <t>103655077.00</t>
-  </si>
-  <si>
-    <t>2056000.00</t>
-  </si>
-  <si>
-    <t>88499437.00</t>
-  </si>
-  <si>
-    <t>159068243.00</t>
-  </si>
-  <si>
-    <t>27785208.00</t>
-  </si>
-  <si>
-    <t>31945979.00</t>
-  </si>
-  <si>
-    <t>6180541.00</t>
-  </si>
-  <si>
-    <t>55321896.00</t>
-  </si>
-  <si>
-    <t>7740251.00</t>
-  </si>
-  <si>
-    <t>29609970.00</t>
-  </si>
-  <si>
-    <t>29179890.00</t>
-  </si>
-  <si>
-    <t>4890364.00</t>
-  </si>
-  <si>
-    <t>33690661.00</t>
-  </si>
-  <si>
-    <t>9679859.00</t>
-  </si>
-  <si>
-    <t>7494508.00</t>
-  </si>
-  <si>
-    <t>700000.00</t>
-  </si>
-  <si>
-    <t>5742520.00</t>
-  </si>
-  <si>
-    <t>223044993.00</t>
-  </si>
-  <si>
-    <t>7564000.00</t>
-  </si>
-  <si>
-    <t>139756795.00</t>
-  </si>
-  <si>
-    <t>284386452.00</t>
-  </si>
-  <si>
-    <t>58361793.00</t>
-  </si>
-  <si>
-    <t>88760577.00</t>
-  </si>
-  <si>
-    <t>5890854.00</t>
-  </si>
-  <si>
-    <t>47245789.00</t>
-  </si>
-  <si>
-    <t>9613708.00</t>
-  </si>
-  <si>
-    <t>47347226.00</t>
-  </si>
-  <si>
-    <t>21662068.00</t>
-  </si>
-  <si>
-    <t>6534259.00</t>
-  </si>
-  <si>
-    <t>38796984.00</t>
-  </si>
-  <si>
-    <t>15126914.00</t>
-  </si>
-  <si>
-    <t>12751832.00</t>
-  </si>
-  <si>
-    <t>2288000.00</t>
-  </si>
-  <si>
-    <t>9328825.00</t>
-  </si>
-  <si>
-    <t>92762230.00</t>
-  </si>
-  <si>
-    <t>720898.00</t>
-  </si>
-  <si>
-    <t>43688264.00</t>
-  </si>
-  <si>
-    <t>102603673.00</t>
-  </si>
-  <si>
-    <t>8131180.00</t>
-  </si>
-  <si>
-    <t>37077612.00</t>
-  </si>
-  <si>
-    <t>3183160.00</t>
-  </si>
-  <si>
-    <t>65432830.00</t>
-  </si>
-  <si>
-    <t>8022840.00</t>
-  </si>
-  <si>
-    <t>18443424.00</t>
-  </si>
-  <si>
-    <t>6106728.00</t>
-  </si>
-  <si>
-    <t>10127359.00</t>
-  </si>
-  <si>
-    <t>16115000.00</t>
-  </si>
-  <si>
-    <t>8818400.00</t>
-  </si>
-  <si>
-    <t>5263308.00</t>
-  </si>
-  <si>
-    <t>697000.00</t>
-  </si>
-  <si>
-    <t>14035102.00</t>
-  </si>
-  <si>
-    <t>2350000.00</t>
-  </si>
-  <si>
-    <t>76568063.00</t>
-  </si>
-  <si>
-    <t>793343.00</t>
-  </si>
-  <si>
-    <t>4517000.00</t>
-  </si>
-  <si>
-    <t>93471025.00</t>
-  </si>
-  <si>
-    <t>330513760.00</t>
-  </si>
-  <si>
-    <t>94085244.00</t>
-  </si>
-  <si>
-    <t>46244692.00</t>
-  </si>
-  <si>
-    <t>10822326.00</t>
-  </si>
-  <si>
-    <t>35235230.00</t>
-  </si>
-  <si>
-    <t>5089773.00</t>
-  </si>
-  <si>
-    <t>96547076.00</t>
-  </si>
-  <si>
-    <t>29748444.00</t>
-  </si>
-  <si>
-    <t>8913852.00</t>
-  </si>
-  <si>
-    <t>28820755.00</t>
-  </si>
-  <si>
-    <t>7455107.00</t>
-  </si>
-  <si>
-    <t>10103771.00</t>
-  </si>
-  <si>
-    <t>287500.00</t>
-  </si>
-  <si>
-    <t>1230800.00</t>
-  </si>
-  <si>
-    <t>849000.00</t>
-  </si>
-  <si>
-    <t>13498461.00</t>
-  </si>
-  <si>
-    <t>11612170.00</t>
-  </si>
-  <si>
-    <t>43888731.00</t>
-  </si>
-  <si>
-    <t>20987900.00</t>
-  </si>
-  <si>
-    <t>5328500.00</t>
-  </si>
-  <si>
-    <t>2031700.00</t>
-  </si>
-  <si>
-    <t>1922000.00</t>
-  </si>
-  <si>
-    <t>2641349.00</t>
-  </si>
-  <si>
-    <t>6120100.00</t>
-  </si>
-  <si>
-    <t>7327053.00</t>
-  </si>
-  <si>
-    <t>1539200.00</t>
-  </si>
-  <si>
-    <t>4152549.00</t>
-  </si>
-  <si>
-    <t>968000.00</t>
-  </si>
-  <si>
-    <t>1328600.00</t>
   </si>
   <si>
     <t>599000.00</t>
@@ -31878,7 +31878,7 @@
         <v>10</v>
       </c>
       <c r="B737" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C737" t="s">
         <v>1385</v>
@@ -31910,7 +31910,7 @@
         <v>10</v>
       </c>
       <c r="B738" t="s">
-        <v>370</v>
+        <v>30</v>
       </c>
       <c r="C738" t="s">
         <v>1386</v>
@@ -31928,10 +31928,10 @@
         <v>2418</v>
       </c>
       <c r="H738" t="s">
-        <v>2610</v>
+        <v>2626</v>
       </c>
       <c r="I738" t="s">
-        <v>2629</v>
+        <v>2645</v>
       </c>
       <c r="J738" t="s">
         <v>2647</v>
@@ -31942,7 +31942,7 @@
         <v>10</v>
       </c>
       <c r="B739" t="s">
-        <v>86</v>
+        <v>240</v>
       </c>
       <c r="C739" t="s">
         <v>1387</v>
@@ -31960,10 +31960,10 @@
         <v>2418</v>
       </c>
       <c r="H739" t="s">
-        <v>2627</v>
+        <v>2610</v>
       </c>
       <c r="I739" t="s">
-        <v>2646</v>
+        <v>2629</v>
       </c>
       <c r="J739" t="s">
         <v>2647</v>
@@ -31974,7 +31974,7 @@
         <v>10</v>
       </c>
       <c r="B740" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="C740" t="s">
         <v>1388</v>
@@ -31992,10 +31992,10 @@
         <v>2418</v>
       </c>
       <c r="H740" t="s">
-        <v>2611</v>
+        <v>2612</v>
       </c>
       <c r="I740" t="s">
-        <v>2630</v>
+        <v>2631</v>
       </c>
       <c r="J740" t="s">
         <v>2647</v>
@@ -32006,7 +32006,7 @@
         <v>10</v>
       </c>
       <c r="B741" t="s">
-        <v>24</v>
+        <v>370</v>
       </c>
       <c r="C741" t="s">
         <v>1389</v>
@@ -32024,10 +32024,10 @@
         <v>2418</v>
       </c>
       <c r="H741" t="s">
-        <v>2612</v>
+        <v>2613</v>
       </c>
       <c r="I741" t="s">
-        <v>2631</v>
+        <v>2632</v>
       </c>
       <c r="J741" t="s">
         <v>2647</v>
@@ -32038,7 +32038,7 @@
         <v>10</v>
       </c>
       <c r="B742" t="s">
-        <v>158</v>
+        <v>95</v>
       </c>
       <c r="C742" t="s">
         <v>1390</v>
@@ -32056,10 +32056,10 @@
         <v>2418</v>
       </c>
       <c r="H742" t="s">
-        <v>2613</v>
+        <v>2614</v>
       </c>
       <c r="I742" t="s">
-        <v>2632</v>
+        <v>2633</v>
       </c>
       <c r="J742" t="s">
         <v>2647</v>
@@ -32070,7 +32070,7 @@
         <v>10</v>
       </c>
       <c r="B743" t="s">
-        <v>371</v>
+        <v>112</v>
       </c>
       <c r="C743" t="s">
         <v>1391</v>
@@ -32088,10 +32088,10 @@
         <v>2418</v>
       </c>
       <c r="H743" t="s">
-        <v>2614</v>
+        <v>2615</v>
       </c>
       <c r="I743" t="s">
-        <v>2633</v>
+        <v>2634</v>
       </c>
       <c r="J743" t="s">
         <v>2647</v>
@@ -32102,7 +32102,7 @@
         <v>10</v>
       </c>
       <c r="B744" t="s">
-        <v>372</v>
+        <v>66</v>
       </c>
       <c r="C744" t="s">
         <v>1392</v>
@@ -32120,10 +32120,10 @@
         <v>2418</v>
       </c>
       <c r="H744" t="s">
-        <v>2615</v>
+        <v>2616</v>
       </c>
       <c r="I744" t="s">
-        <v>2634</v>
+        <v>2635</v>
       </c>
       <c r="J744" t="s">
         <v>2647</v>
@@ -32134,7 +32134,7 @@
         <v>10</v>
       </c>
       <c r="B745" t="s">
-        <v>346</v>
+        <v>62</v>
       </c>
       <c r="C745" t="s">
         <v>1393</v>
@@ -32152,10 +32152,10 @@
         <v>2418</v>
       </c>
       <c r="H745" t="s">
-        <v>2616</v>
+        <v>2617</v>
       </c>
       <c r="I745" t="s">
-        <v>2635</v>
+        <v>2636</v>
       </c>
       <c r="J745" t="s">
         <v>2647</v>
@@ -32166,7 +32166,7 @@
         <v>10</v>
       </c>
       <c r="B746" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="C746" t="s">
         <v>1394</v>
@@ -32184,10 +32184,10 @@
         <v>2418</v>
       </c>
       <c r="H746" t="s">
-        <v>2617</v>
+        <v>2618</v>
       </c>
       <c r="I746" t="s">
-        <v>2636</v>
+        <v>2637</v>
       </c>
       <c r="J746" t="s">
         <v>2647</v>
@@ -32198,7 +32198,7 @@
         <v>10</v>
       </c>
       <c r="B747" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="C747" t="s">
         <v>1395</v>
@@ -32216,10 +32216,10 @@
         <v>2418</v>
       </c>
       <c r="H747" t="s">
-        <v>2618</v>
+        <v>2619</v>
       </c>
       <c r="I747" t="s">
-        <v>2637</v>
+        <v>2638</v>
       </c>
       <c r="J747" t="s">
         <v>2647</v>
@@ -32230,7 +32230,7 @@
         <v>10</v>
       </c>
       <c r="B748" t="s">
-        <v>373</v>
+        <v>84</v>
       </c>
       <c r="C748" t="s">
         <v>1396</v>
@@ -32248,10 +32248,10 @@
         <v>2418</v>
       </c>
       <c r="H748" t="s">
-        <v>2619</v>
+        <v>2620</v>
       </c>
       <c r="I748" t="s">
-        <v>2638</v>
+        <v>2639</v>
       </c>
       <c r="J748" t="s">
         <v>2647</v>
@@ -32262,7 +32262,7 @@
         <v>10</v>
       </c>
       <c r="B749" t="s">
-        <v>326</v>
+        <v>27</v>
       </c>
       <c r="C749" t="s">
         <v>1397</v>
@@ -32280,10 +32280,10 @@
         <v>2418</v>
       </c>
       <c r="H749" t="s">
-        <v>2620</v>
+        <v>2621</v>
       </c>
       <c r="I749" t="s">
-        <v>2639</v>
+        <v>2640</v>
       </c>
       <c r="J749" t="s">
         <v>2647</v>
@@ -32294,7 +32294,7 @@
         <v>10</v>
       </c>
       <c r="B750" t="s">
-        <v>18</v>
+        <v>169</v>
       </c>
       <c r="C750" t="s">
         <v>1398</v>
@@ -32312,10 +32312,10 @@
         <v>2418</v>
       </c>
       <c r="H750" t="s">
-        <v>2621</v>
+        <v>2622</v>
       </c>
       <c r="I750" t="s">
-        <v>2640</v>
+        <v>2641</v>
       </c>
       <c r="J750" t="s">
         <v>2647</v>
@@ -32326,7 +32326,7 @@
         <v>10</v>
       </c>
       <c r="B751" t="s">
-        <v>352</v>
+        <v>13</v>
       </c>
       <c r="C751" t="s">
         <v>1399</v>
@@ -32344,10 +32344,10 @@
         <v>2418</v>
       </c>
       <c r="H751" t="s">
-        <v>2622</v>
+        <v>2623</v>
       </c>
       <c r="I751" t="s">
-        <v>2641</v>
+        <v>2642</v>
       </c>
       <c r="J751" t="s">
         <v>2647</v>
@@ -32358,7 +32358,7 @@
         <v>10</v>
       </c>
       <c r="B752" t="s">
-        <v>363</v>
+        <v>33</v>
       </c>
       <c r="C752" t="s">
         <v>1400</v>
@@ -32376,10 +32376,10 @@
         <v>2418</v>
       </c>
       <c r="H752" t="s">
-        <v>2623</v>
+        <v>2624</v>
       </c>
       <c r="I752" t="s">
-        <v>2642</v>
+        <v>2643</v>
       </c>
       <c r="J752" t="s">
         <v>2647</v>
@@ -32390,28 +32390,28 @@
         <v>10</v>
       </c>
       <c r="B753" t="s">
-        <v>371</v>
+        <v>240</v>
       </c>
       <c r="C753" t="s">
         <v>1401</v>
       </c>
       <c r="D753" t="s">
-        <v>2400</v>
+        <v>2401</v>
       </c>
       <c r="E753" t="s">
-        <v>2418</v>
+        <v>2419</v>
       </c>
       <c r="F753" t="s">
-        <v>2468</v>
+        <v>2403</v>
       </c>
       <c r="G753" t="s">
-        <v>2418</v>
+        <v>2555</v>
       </c>
       <c r="H753" t="s">
-        <v>2624</v>
+        <v>2609</v>
       </c>
       <c r="I753" t="s">
-        <v>2643</v>
+        <v>2628</v>
       </c>
       <c r="J753" t="s">
         <v>2647</v>
@@ -32422,28 +32422,28 @@
         <v>10</v>
       </c>
       <c r="B754" t="s">
-        <v>99</v>
+        <v>194</v>
       </c>
       <c r="C754" t="s">
         <v>1402</v>
       </c>
       <c r="D754" t="s">
-        <v>2400</v>
+        <v>2401</v>
       </c>
       <c r="E754" t="s">
-        <v>2418</v>
+        <v>2419</v>
       </c>
       <c r="F754" t="s">
-        <v>2468</v>
+        <v>2403</v>
       </c>
       <c r="G754" t="s">
-        <v>2418</v>
+        <v>2555</v>
       </c>
       <c r="H754" t="s">
-        <v>2625</v>
+        <v>2610</v>
       </c>
       <c r="I754" t="s">
-        <v>2644</v>
+        <v>2629</v>
       </c>
       <c r="J754" t="s">
         <v>2647</v>
@@ -32454,7 +32454,7 @@
         <v>10</v>
       </c>
       <c r="B755" t="s">
-        <v>240</v>
+        <v>68</v>
       </c>
       <c r="C755" t="s">
         <v>1403</v>
@@ -32472,10 +32472,10 @@
         <v>2555</v>
       </c>
       <c r="H755" t="s">
-        <v>2609</v>
+        <v>2611</v>
       </c>
       <c r="I755" t="s">
-        <v>2628</v>
+        <v>2630</v>
       </c>
       <c r="J755" t="s">
         <v>2647</v>
@@ -32486,7 +32486,7 @@
         <v>10</v>
       </c>
       <c r="B756" t="s">
-        <v>194</v>
+        <v>371</v>
       </c>
       <c r="C756" t="s">
         <v>1404</v>
@@ -32504,10 +32504,10 @@
         <v>2555</v>
       </c>
       <c r="H756" t="s">
-        <v>2610</v>
+        <v>2612</v>
       </c>
       <c r="I756" t="s">
-        <v>2629</v>
+        <v>2631</v>
       </c>
       <c r="J756" t="s">
         <v>2647</v>
@@ -32518,7 +32518,7 @@
         <v>10</v>
       </c>
       <c r="B757" t="s">
-        <v>68</v>
+        <v>372</v>
       </c>
       <c r="C757" t="s">
         <v>1405</v>
@@ -32536,10 +32536,10 @@
         <v>2555</v>
       </c>
       <c r="H757" t="s">
-        <v>2611</v>
+        <v>2613</v>
       </c>
       <c r="I757" t="s">
-        <v>2630</v>
+        <v>2632</v>
       </c>
       <c r="J757" t="s">
         <v>2647</v>
@@ -32550,7 +32550,7 @@
         <v>10</v>
       </c>
       <c r="B758" t="s">
-        <v>374</v>
+        <v>11</v>
       </c>
       <c r="C758" t="s">
         <v>1406</v>
@@ -32568,10 +32568,10 @@
         <v>2555</v>
       </c>
       <c r="H758" t="s">
-        <v>2612</v>
+        <v>2614</v>
       </c>
       <c r="I758" t="s">
-        <v>2631</v>
+        <v>2633</v>
       </c>
       <c r="J758" t="s">
         <v>2647</v>
@@ -32582,7 +32582,7 @@
         <v>10</v>
       </c>
       <c r="B759" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C759" t="s">
         <v>1407</v>
@@ -32600,10 +32600,10 @@
         <v>2555</v>
       </c>
       <c r="H759" t="s">
-        <v>2613</v>
+        <v>2615</v>
       </c>
       <c r="I759" t="s">
-        <v>2632</v>
+        <v>2634</v>
       </c>
       <c r="J759" t="s">
         <v>2647</v>
@@ -32614,7 +32614,7 @@
         <v>10</v>
       </c>
       <c r="B760" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="C760" t="s">
         <v>1408</v>
@@ -32632,10 +32632,10 @@
         <v>2555</v>
       </c>
       <c r="H760" t="s">
-        <v>2614</v>
+        <v>2616</v>
       </c>
       <c r="I760" t="s">
-        <v>2633</v>
+        <v>2635</v>
       </c>
       <c r="J760" t="s">
         <v>2647</v>
@@ -32646,7 +32646,7 @@
         <v>10</v>
       </c>
       <c r="B761" t="s">
-        <v>376</v>
+        <v>52</v>
       </c>
       <c r="C761" t="s">
         <v>1409</v>
@@ -32664,10 +32664,10 @@
         <v>2555</v>
       </c>
       <c r="H761" t="s">
-        <v>2615</v>
+        <v>2617</v>
       </c>
       <c r="I761" t="s">
-        <v>2634</v>
+        <v>2636</v>
       </c>
       <c r="J761" t="s">
         <v>2647</v>
@@ -32678,7 +32678,7 @@
         <v>10</v>
       </c>
       <c r="B762" t="s">
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="C762" t="s">
         <v>1410</v>
@@ -32696,10 +32696,10 @@
         <v>2555</v>
       </c>
       <c r="H762" t="s">
-        <v>2616</v>
+        <v>2618</v>
       </c>
       <c r="I762" t="s">
-        <v>2635</v>
+        <v>2637</v>
       </c>
       <c r="J762" t="s">
         <v>2647</v>
@@ -32710,7 +32710,7 @@
         <v>10</v>
       </c>
       <c r="B763" t="s">
-        <v>52</v>
+        <v>230</v>
       </c>
       <c r="C763" t="s">
         <v>1411</v>
@@ -32728,10 +32728,10 @@
         <v>2555</v>
       </c>
       <c r="H763" t="s">
-        <v>2617</v>
+        <v>2619</v>
       </c>
       <c r="I763" t="s">
-        <v>2636</v>
+        <v>2638</v>
       </c>
       <c r="J763" t="s">
         <v>2647</v>
@@ -32742,7 +32742,7 @@
         <v>10</v>
       </c>
       <c r="B764" t="s">
-        <v>188</v>
+        <v>76</v>
       </c>
       <c r="C764" t="s">
         <v>1412</v>
@@ -32760,10 +32760,10 @@
         <v>2555</v>
       </c>
       <c r="H764" t="s">
-        <v>2618</v>
+        <v>2620</v>
       </c>
       <c r="I764" t="s">
-        <v>2637</v>
+        <v>2639</v>
       </c>
       <c r="J764" t="s">
         <v>2647</v>
@@ -32774,7 +32774,7 @@
         <v>10</v>
       </c>
       <c r="B765" t="s">
-        <v>230</v>
+        <v>94</v>
       </c>
       <c r="C765" t="s">
         <v>1413</v>
@@ -32792,10 +32792,10 @@
         <v>2555</v>
       </c>
       <c r="H765" t="s">
-        <v>2619</v>
+        <v>2621</v>
       </c>
       <c r="I765" t="s">
-        <v>2638</v>
+        <v>2640</v>
       </c>
       <c r="J765" t="s">
         <v>2647</v>
@@ -32806,7 +32806,7 @@
         <v>10</v>
       </c>
       <c r="B766" t="s">
-        <v>76</v>
+        <v>287</v>
       </c>
       <c r="C766" t="s">
         <v>1414</v>
@@ -32824,10 +32824,10 @@
         <v>2555</v>
       </c>
       <c r="H766" t="s">
-        <v>2620</v>
+        <v>2622</v>
       </c>
       <c r="I766" t="s">
-        <v>2639</v>
+        <v>2641</v>
       </c>
       <c r="J766" t="s">
         <v>2647</v>
@@ -32838,7 +32838,7 @@
         <v>10</v>
       </c>
       <c r="B767" t="s">
-        <v>94</v>
+        <v>364</v>
       </c>
       <c r="C767" t="s">
         <v>1415</v>
@@ -32856,10 +32856,10 @@
         <v>2555</v>
       </c>
       <c r="H767" t="s">
-        <v>2621</v>
+        <v>2623</v>
       </c>
       <c r="I767" t="s">
-        <v>2640</v>
+        <v>2642</v>
       </c>
       <c r="J767" t="s">
         <v>2647</v>
@@ -32870,7 +32870,7 @@
         <v>10</v>
       </c>
       <c r="B768" t="s">
-        <v>287</v>
+        <v>43</v>
       </c>
       <c r="C768" t="s">
         <v>1416</v>
@@ -32888,10 +32888,10 @@
         <v>2555</v>
       </c>
       <c r="H768" t="s">
-        <v>2622</v>
+        <v>2624</v>
       </c>
       <c r="I768" t="s">
-        <v>2641</v>
+        <v>2643</v>
       </c>
       <c r="J768" t="s">
         <v>2647</v>
@@ -32902,7 +32902,7 @@
         <v>10</v>
       </c>
       <c r="B769" t="s">
-        <v>364</v>
+        <v>13</v>
       </c>
       <c r="C769" t="s">
         <v>1417</v>
@@ -32920,10 +32920,10 @@
         <v>2555</v>
       </c>
       <c r="H769" t="s">
-        <v>2623</v>
+        <v>2625</v>
       </c>
       <c r="I769" t="s">
-        <v>2642</v>
+        <v>2644</v>
       </c>
       <c r="J769" t="s">
         <v>2647</v>
@@ -32934,7 +32934,7 @@
         <v>10</v>
       </c>
       <c r="B770" t="s">
-        <v>43</v>
+        <v>326</v>
       </c>
       <c r="C770" t="s">
         <v>1418</v>
@@ -32946,16 +32946,16 @@
         <v>2419</v>
       </c>
       <c r="F770" t="s">
-        <v>2403</v>
+        <v>2469</v>
       </c>
       <c r="G770" t="s">
-        <v>2555</v>
+        <v>2556</v>
       </c>
       <c r="H770" t="s">
-        <v>2624</v>
+        <v>2609</v>
       </c>
       <c r="I770" t="s">
-        <v>2643</v>
+        <v>2628</v>
       </c>
       <c r="J770" t="s">
         <v>2647</v>
@@ -32966,7 +32966,7 @@
         <v>10</v>
       </c>
       <c r="B771" t="s">
-        <v>13</v>
+        <v>374</v>
       </c>
       <c r="C771" t="s">
         <v>1419</v>
@@ -32978,16 +32978,16 @@
         <v>2419</v>
       </c>
       <c r="F771" t="s">
-        <v>2403</v>
+        <v>2469</v>
       </c>
       <c r="G771" t="s">
-        <v>2555</v>
+        <v>2556</v>
       </c>
       <c r="H771" t="s">
-        <v>2625</v>
+        <v>2610</v>
       </c>
       <c r="I771" t="s">
-        <v>2644</v>
+        <v>2629</v>
       </c>
       <c r="J771" t="s">
         <v>2647</v>
@@ -32998,7 +32998,7 @@
         <v>10</v>
       </c>
       <c r="B772" t="s">
-        <v>326</v>
+        <v>30</v>
       </c>
       <c r="C772" t="s">
         <v>1420</v>
@@ -33016,10 +33016,10 @@
         <v>2556</v>
       </c>
       <c r="H772" t="s">
-        <v>2609</v>
+        <v>2627</v>
       </c>
       <c r="I772" t="s">
-        <v>2628</v>
+        <v>2646</v>
       </c>
       <c r="J772" t="s">
         <v>2647</v>
@@ -33030,7 +33030,7 @@
         <v>10</v>
       </c>
       <c r="B773" t="s">
-        <v>377</v>
+        <v>19</v>
       </c>
       <c r="C773" t="s">
         <v>1421</v>
@@ -33048,10 +33048,10 @@
         <v>2556</v>
       </c>
       <c r="H773" t="s">
-        <v>2610</v>
+        <v>2611</v>
       </c>
       <c r="I773" t="s">
-        <v>2629</v>
+        <v>2630</v>
       </c>
       <c r="J773" t="s">
         <v>2647</v>
@@ -33062,7 +33062,7 @@
         <v>10</v>
       </c>
       <c r="B774" t="s">
-        <v>30</v>
+        <v>375</v>
       </c>
       <c r="C774" t="s">
         <v>1422</v>
@@ -33080,10 +33080,10 @@
         <v>2556</v>
       </c>
       <c r="H774" t="s">
-        <v>2627</v>
+        <v>2612</v>
       </c>
       <c r="I774" t="s">
-        <v>2646</v>
+        <v>2631</v>
       </c>
       <c r="J774" t="s">
         <v>2647</v>
@@ -33094,7 +33094,7 @@
         <v>10</v>
       </c>
       <c r="B775" t="s">
-        <v>19</v>
+        <v>376</v>
       </c>
       <c r="C775" t="s">
         <v>1423</v>
@@ -33112,10 +33112,10 @@
         <v>2556</v>
       </c>
       <c r="H775" t="s">
-        <v>2611</v>
+        <v>2613</v>
       </c>
       <c r="I775" t="s">
-        <v>2630</v>
+        <v>2632</v>
       </c>
       <c r="J775" t="s">
         <v>2647</v>
@@ -33126,7 +33126,7 @@
         <v>10</v>
       </c>
       <c r="B776" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C776" t="s">
         <v>1424</v>
@@ -33144,10 +33144,10 @@
         <v>2556</v>
       </c>
       <c r="H776" t="s">
-        <v>2612</v>
+        <v>2614</v>
       </c>
       <c r="I776" t="s">
-        <v>2631</v>
+        <v>2633</v>
       </c>
       <c r="J776" t="s">
         <v>2647</v>
@@ -33158,7 +33158,7 @@
         <v>10</v>
       </c>
       <c r="B777" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C777" t="s">
         <v>1425</v>
@@ -33176,10 +33176,10 @@
         <v>2556</v>
       </c>
       <c r="H777" t="s">
-        <v>2613</v>
+        <v>2615</v>
       </c>
       <c r="I777" t="s">
-        <v>2632</v>
+        <v>2634</v>
       </c>
       <c r="J777" t="s">
         <v>2647</v>
@@ -33190,7 +33190,7 @@
         <v>10</v>
       </c>
       <c r="B778" t="s">
-        <v>380</v>
+        <v>159</v>
       </c>
       <c r="C778" t="s">
         <v>1426</v>
@@ -33208,10 +33208,10 @@
         <v>2556</v>
       </c>
       <c r="H778" t="s">
-        <v>2614</v>
+        <v>2616</v>
       </c>
       <c r="I778" t="s">
-        <v>2633</v>
+        <v>2635</v>
       </c>
       <c r="J778" t="s">
         <v>2647</v>
@@ -33222,7 +33222,7 @@
         <v>10</v>
       </c>
       <c r="B779" t="s">
-        <v>381</v>
+        <v>193</v>
       </c>
       <c r="C779" t="s">
         <v>1427</v>
@@ -33240,10 +33240,10 @@
         <v>2556</v>
       </c>
       <c r="H779" t="s">
-        <v>2615</v>
+        <v>2617</v>
       </c>
       <c r="I779" t="s">
-        <v>2634</v>
+        <v>2636</v>
       </c>
       <c r="J779" t="s">
         <v>2647</v>
@@ -33254,7 +33254,7 @@
         <v>10</v>
       </c>
       <c r="B780" t="s">
-        <v>159</v>
+        <v>283</v>
       </c>
       <c r="C780" t="s">
         <v>1428</v>
@@ -33272,10 +33272,10 @@
         <v>2556</v>
       </c>
       <c r="H780" t="s">
-        <v>2616</v>
+        <v>2618</v>
       </c>
       <c r="I780" t="s">
-        <v>2635</v>
+        <v>2637</v>
       </c>
       <c r="J780" t="s">
         <v>2647</v>
@@ -33286,7 +33286,7 @@
         <v>10</v>
       </c>
       <c r="B781" t="s">
-        <v>193</v>
+        <v>379</v>
       </c>
       <c r="C781" t="s">
         <v>1429</v>
@@ -33304,10 +33304,10 @@
         <v>2556</v>
       </c>
       <c r="H781" t="s">
-        <v>2617</v>
+        <v>2619</v>
       </c>
       <c r="I781" t="s">
-        <v>2636</v>
+        <v>2638</v>
       </c>
       <c r="J781" t="s">
         <v>2647</v>
@@ -33318,7 +33318,7 @@
         <v>10</v>
       </c>
       <c r="B782" t="s">
-        <v>283</v>
+        <v>360</v>
       </c>
       <c r="C782" t="s">
         <v>1430</v>
@@ -33336,10 +33336,10 @@
         <v>2556</v>
       </c>
       <c r="H782" t="s">
-        <v>2618</v>
+        <v>2620</v>
       </c>
       <c r="I782" t="s">
-        <v>2637</v>
+        <v>2639</v>
       </c>
       <c r="J782" t="s">
         <v>2647</v>
@@ -33350,7 +33350,7 @@
         <v>10</v>
       </c>
       <c r="B783" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C783" t="s">
         <v>1431</v>
@@ -33368,10 +33368,10 @@
         <v>2556</v>
       </c>
       <c r="H783" t="s">
-        <v>2619</v>
+        <v>2621</v>
       </c>
       <c r="I783" t="s">
-        <v>2638</v>
+        <v>2640</v>
       </c>
       <c r="J783" t="s">
         <v>2647</v>
@@ -33382,7 +33382,7 @@
         <v>10</v>
       </c>
       <c r="B784" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="C784" t="s">
         <v>1432</v>
@@ -33400,10 +33400,10 @@
         <v>2556</v>
       </c>
       <c r="H784" t="s">
-        <v>2620</v>
+        <v>2622</v>
       </c>
       <c r="I784" t="s">
-        <v>2639</v>
+        <v>2641</v>
       </c>
       <c r="J784" t="s">
         <v>2647</v>
@@ -33414,7 +33414,7 @@
         <v>10</v>
       </c>
       <c r="B785" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C785" t="s">
         <v>1433</v>
@@ -33432,10 +33432,10 @@
         <v>2556</v>
       </c>
       <c r="H785" t="s">
-        <v>2621</v>
+        <v>2623</v>
       </c>
       <c r="I785" t="s">
-        <v>2640</v>
+        <v>2642</v>
       </c>
       <c r="J785" t="s">
         <v>2647</v>
@@ -33446,7 +33446,7 @@
         <v>10</v>
       </c>
       <c r="B786" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C786" t="s">
         <v>1434</v>
@@ -33464,10 +33464,10 @@
         <v>2556</v>
       </c>
       <c r="H786" t="s">
-        <v>2622</v>
+        <v>2624</v>
       </c>
       <c r="I786" t="s">
-        <v>2641</v>
+        <v>2643</v>
       </c>
       <c r="J786" t="s">
         <v>2647</v>
@@ -33478,7 +33478,7 @@
         <v>10</v>
       </c>
       <c r="B787" t="s">
-        <v>372</v>
+        <v>56</v>
       </c>
       <c r="C787" t="s">
         <v>1435</v>
@@ -33496,10 +33496,10 @@
         <v>2556</v>
       </c>
       <c r="H787" t="s">
-        <v>2623</v>
+        <v>2625</v>
       </c>
       <c r="I787" t="s">
-        <v>2642</v>
+        <v>2644</v>
       </c>
       <c r="J787" t="s">
         <v>2647</v>
@@ -33510,7 +33510,7 @@
         <v>10</v>
       </c>
       <c r="B788" t="s">
-        <v>385</v>
+        <v>134</v>
       </c>
       <c r="C788" t="s">
         <v>1436</v>
@@ -33522,16 +33522,16 @@
         <v>2419</v>
       </c>
       <c r="F788" t="s">
-        <v>2469</v>
+        <v>2470</v>
       </c>
       <c r="G788" t="s">
-        <v>2556</v>
+        <v>2557</v>
       </c>
       <c r="H788" t="s">
-        <v>2624</v>
+        <v>2609</v>
       </c>
       <c r="I788" t="s">
-        <v>2643</v>
+        <v>2628</v>
       </c>
       <c r="J788" t="s">
         <v>2647</v>
@@ -33542,7 +33542,7 @@
         <v>10</v>
       </c>
       <c r="B789" t="s">
-        <v>56</v>
+        <v>304</v>
       </c>
       <c r="C789" t="s">
         <v>1437</v>
@@ -33554,16 +33554,16 @@
         <v>2419</v>
       </c>
       <c r="F789" t="s">
-        <v>2469</v>
+        <v>2470</v>
       </c>
       <c r="G789" t="s">
-        <v>2556</v>
+        <v>2557</v>
       </c>
       <c r="H789" t="s">
-        <v>2625</v>
+        <v>2610</v>
       </c>
       <c r="I789" t="s">
-        <v>2644</v>
+        <v>2629</v>
       </c>
       <c r="J789" t="s">
         <v>2647</v>
@@ -33574,7 +33574,7 @@
         <v>10</v>
       </c>
       <c r="B790" t="s">
-        <v>134</v>
+        <v>47</v>
       </c>
       <c r="C790" t="s">
         <v>1438</v>
@@ -33592,10 +33592,10 @@
         <v>2557</v>
       </c>
       <c r="H790" t="s">
-        <v>2609</v>
+        <v>2611</v>
       </c>
       <c r="I790" t="s">
-        <v>2628</v>
+        <v>2630</v>
       </c>
       <c r="J790" t="s">
         <v>2647</v>
@@ -33606,7 +33606,7 @@
         <v>10</v>
       </c>
       <c r="B791" t="s">
-        <v>304</v>
+        <v>384</v>
       </c>
       <c r="C791" t="s">
         <v>1439</v>
@@ -33624,10 +33624,10 @@
         <v>2557</v>
       </c>
       <c r="H791" t="s">
-        <v>2610</v>
+        <v>2612</v>
       </c>
       <c r="I791" t="s">
-        <v>2629</v>
+        <v>2631</v>
       </c>
       <c r="J791" t="s">
         <v>2647</v>
@@ -33638,7 +33638,7 @@
         <v>10</v>
       </c>
       <c r="B792" t="s">
-        <v>47</v>
+        <v>385</v>
       </c>
       <c r="C792" t="s">
         <v>1440</v>
@@ -33656,10 +33656,10 @@
         <v>2557</v>
       </c>
       <c r="H792" t="s">
-        <v>2611</v>
+        <v>2613</v>
       </c>
       <c r="I792" t="s">
-        <v>2630</v>
+        <v>2632</v>
       </c>
       <c r="J792" t="s">
         <v>2647</v>
@@ -33670,7 +33670,7 @@
         <v>10</v>
       </c>
       <c r="B793" t="s">
-        <v>386</v>
+        <v>231</v>
       </c>
       <c r="C793" t="s">
         <v>1441</v>
@@ -33688,10 +33688,10 @@
         <v>2557</v>
       </c>
       <c r="H793" t="s">
-        <v>2612</v>
+        <v>2614</v>
       </c>
       <c r="I793" t="s">
-        <v>2631</v>
+        <v>2633</v>
       </c>
       <c r="J793" t="s">
         <v>2647</v>
@@ -33702,7 +33702,7 @@
         <v>10</v>
       </c>
       <c r="B794" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C794" t="s">
         <v>1442</v>
@@ -33720,10 +33720,10 @@
         <v>2557</v>
       </c>
       <c r="H794" t="s">
-        <v>2613</v>
+        <v>2615</v>
       </c>
       <c r="I794" t="s">
-        <v>2632</v>
+        <v>2634</v>
       </c>
       <c r="J794" t="s">
         <v>2647</v>
@@ -33734,7 +33734,7 @@
         <v>10</v>
       </c>
       <c r="B795" t="s">
-        <v>231</v>
+        <v>98</v>
       </c>
       <c r="C795" t="s">
         <v>1443</v>
@@ -33752,10 +33752,10 @@
         <v>2557</v>
       </c>
       <c r="H795" t="s">
-        <v>2614</v>
+        <v>2616</v>
       </c>
       <c r="I795" t="s">
-        <v>2633</v>
+        <v>2635</v>
       </c>
       <c r="J795" t="s">
         <v>2647</v>
@@ -33766,7 +33766,7 @@
         <v>10</v>
       </c>
       <c r="B796" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C796" t="s">
         <v>1444</v>
@@ -33784,10 +33784,10 @@
         <v>2557</v>
       </c>
       <c r="H796" t="s">
-        <v>2615</v>
+        <v>2617</v>
       </c>
       <c r="I796" t="s">
-        <v>2634</v>
+        <v>2636</v>
       </c>
       <c r="J796" t="s">
         <v>2647</v>
@@ -33798,7 +33798,7 @@
         <v>10</v>
       </c>
       <c r="B797" t="s">
-        <v>98</v>
+        <v>388</v>
       </c>
       <c r="C797" t="s">
         <v>1445</v>
@@ -33816,10 +33816,10 @@
         <v>2557</v>
       </c>
       <c r="H797" t="s">
-        <v>2616</v>
+        <v>2618</v>
       </c>
       <c r="I797" t="s">
-        <v>2635</v>
+        <v>2637</v>
       </c>
       <c r="J797" t="s">
         <v>2647</v>
@@ -33830,7 +33830,7 @@
         <v>10</v>
       </c>
       <c r="B798" t="s">
-        <v>389</v>
+        <v>191</v>
       </c>
       <c r="C798" t="s">
         <v>1446</v>
@@ -33848,10 +33848,10 @@
         <v>2557</v>
       </c>
       <c r="H798" t="s">
-        <v>2617</v>
+        <v>2619</v>
       </c>
       <c r="I798" t="s">
-        <v>2636</v>
+        <v>2638</v>
       </c>
       <c r="J798" t="s">
         <v>2647</v>
@@ -33862,7 +33862,7 @@
         <v>10</v>
       </c>
       <c r="B799" t="s">
-        <v>390</v>
+        <v>43</v>
       </c>
       <c r="C799" t="s">
         <v>1447</v>
@@ -33880,10 +33880,10 @@
         <v>2557</v>
       </c>
       <c r="H799" t="s">
-        <v>2618</v>
+        <v>2620</v>
       </c>
       <c r="I799" t="s">
-        <v>2637</v>
+        <v>2639</v>
       </c>
       <c r="J799" t="s">
         <v>2647</v>
@@ -33894,7 +33894,7 @@
         <v>10</v>
       </c>
       <c r="B800" t="s">
-        <v>191</v>
+        <v>135</v>
       </c>
       <c r="C800" t="s">
         <v>1448</v>
@@ -33912,10 +33912,10 @@
         <v>2557</v>
       </c>
       <c r="H800" t="s">
-        <v>2619</v>
+        <v>2621</v>
       </c>
       <c r="I800" t="s">
-        <v>2638</v>
+        <v>2640</v>
       </c>
       <c r="J800" t="s">
         <v>2647</v>
@@ -33926,7 +33926,7 @@
         <v>10</v>
       </c>
       <c r="B801" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="C801" t="s">
         <v>1449</v>
@@ -33944,10 +33944,10 @@
         <v>2557</v>
       </c>
       <c r="H801" t="s">
-        <v>2620</v>
+        <v>2622</v>
       </c>
       <c r="I801" t="s">
-        <v>2639</v>
+        <v>2641</v>
       </c>
       <c r="J801" t="s">
         <v>2647</v>
@@ -33958,7 +33958,7 @@
         <v>10</v>
       </c>
       <c r="B802" t="s">
-        <v>135</v>
+        <v>350</v>
       </c>
       <c r="C802" t="s">
         <v>1450</v>
@@ -33976,10 +33976,10 @@
         <v>2557</v>
       </c>
       <c r="H802" t="s">
-        <v>2621</v>
+        <v>2623</v>
       </c>
       <c r="I802" t="s">
-        <v>2640</v>
+        <v>2642</v>
       </c>
       <c r="J802" t="s">
         <v>2647</v>
@@ -33990,7 +33990,7 @@
         <v>10</v>
       </c>
       <c r="B803" t="s">
-        <v>90</v>
+        <v>389</v>
       </c>
       <c r="C803" t="s">
         <v>1451</v>
@@ -34008,10 +34008,10 @@
         <v>2557</v>
       </c>
       <c r="H803" t="s">
-        <v>2622</v>
+        <v>2624</v>
       </c>
       <c r="I803" t="s">
-        <v>2641</v>
+        <v>2643</v>
       </c>
       <c r="J803" t="s">
         <v>2647</v>
@@ -34022,7 +34022,7 @@
         <v>10</v>
       </c>
       <c r="B804" t="s">
-        <v>350</v>
+        <v>44</v>
       </c>
       <c r="C804" t="s">
         <v>1452</v>
@@ -34040,10 +34040,10 @@
         <v>2557</v>
       </c>
       <c r="H804" t="s">
-        <v>2623</v>
+        <v>2625</v>
       </c>
       <c r="I804" t="s">
-        <v>2642</v>
+        <v>2644</v>
       </c>
       <c r="J804" t="s">
         <v>2647</v>
@@ -34054,7 +34054,7 @@
         <v>10</v>
       </c>
       <c r="B805" t="s">
-        <v>391</v>
+        <v>263</v>
       </c>
       <c r="C805" t="s">
         <v>1453</v>
@@ -34066,16 +34066,16 @@
         <v>2419</v>
       </c>
       <c r="F805" t="s">
-        <v>2470</v>
+        <v>2471</v>
       </c>
       <c r="G805" t="s">
-        <v>2557</v>
+        <v>2558</v>
       </c>
       <c r="H805" t="s">
-        <v>2624</v>
+        <v>2609</v>
       </c>
       <c r="I805" t="s">
-        <v>2643</v>
+        <v>2628</v>
       </c>
       <c r="J805" t="s">
         <v>2647</v>
@@ -34086,7 +34086,7 @@
         <v>10</v>
       </c>
       <c r="B806" t="s">
-        <v>44</v>
+        <v>185</v>
       </c>
       <c r="C806" t="s">
         <v>1454</v>
@@ -34098,16 +34098,16 @@
         <v>2419</v>
       </c>
       <c r="F806" t="s">
-        <v>2470</v>
+        <v>2471</v>
       </c>
       <c r="G806" t="s">
-        <v>2557</v>
+        <v>2558</v>
       </c>
       <c r="H806" t="s">
-        <v>2625</v>
+        <v>2610</v>
       </c>
       <c r="I806" t="s">
-        <v>2644</v>
+        <v>2629</v>
       </c>
       <c r="J806" t="s">
         <v>2647</v>
@@ -34118,7 +34118,7 @@
         <v>10</v>
       </c>
       <c r="B807" t="s">
-        <v>263</v>
+        <v>92</v>
       </c>
       <c r="C807" t="s">
         <v>1455</v>
@@ -34136,10 +34136,10 @@
         <v>2558</v>
       </c>
       <c r="H807" t="s">
-        <v>2609</v>
+        <v>2611</v>
       </c>
       <c r="I807" t="s">
-        <v>2628</v>
+        <v>2630</v>
       </c>
       <c r="J807" t="s">
         <v>2647</v>
@@ -34150,7 +34150,7 @@
         <v>10</v>
       </c>
       <c r="B808" t="s">
-        <v>185</v>
+        <v>390</v>
       </c>
       <c r="C808" t="s">
         <v>1456</v>
@@ -34168,10 +34168,10 @@
         <v>2558</v>
       </c>
       <c r="H808" t="s">
-        <v>2610</v>
+        <v>2612</v>
       </c>
       <c r="I808" t="s">
-        <v>2629</v>
+        <v>2631</v>
       </c>
       <c r="J808" t="s">
         <v>2647</v>
@@ -34182,7 +34182,7 @@
         <v>10</v>
       </c>
       <c r="B809" t="s">
-        <v>92</v>
+        <v>391</v>
       </c>
       <c r="C809" t="s">
         <v>1457</v>
@@ -34200,10 +34200,10 @@
         <v>2558</v>
       </c>
       <c r="H809" t="s">
-        <v>2611</v>
+        <v>2613</v>
       </c>
       <c r="I809" t="s">
-        <v>2630</v>
+        <v>2632</v>
       </c>
       <c r="J809" t="s">
         <v>2647</v>
@@ -34214,7 +34214,7 @@
         <v>10</v>
       </c>
       <c r="B810" t="s">
-        <v>392</v>
+        <v>327</v>
       </c>
       <c r="C810" t="s">
         <v>1458</v>
@@ -34232,10 +34232,10 @@
         <v>2558</v>
       </c>
       <c r="H810" t="s">
-        <v>2612</v>
+        <v>2614</v>
       </c>
       <c r="I810" t="s">
-        <v>2631</v>
+        <v>2633</v>
       </c>
       <c r="J810" t="s">
         <v>2647</v>
@@ -34246,7 +34246,7 @@
         <v>10</v>
       </c>
       <c r="B811" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C811" t="s">
         <v>1459</v>
@@ -34264,10 +34264,10 @@
         <v>2558</v>
       </c>
       <c r="H811" t="s">
-        <v>2613</v>
+        <v>2615</v>
       </c>
       <c r="I811" t="s">
-        <v>2632</v>
+        <v>2634</v>
       </c>
       <c r="J811" t="s">
         <v>2647</v>
@@ -34278,7 +34278,7 @@
         <v>10</v>
       </c>
       <c r="B812" t="s">
-        <v>327</v>
+        <v>76</v>
       </c>
       <c r="C812" t="s">
         <v>1460</v>
@@ -34296,10 +34296,10 @@
         <v>2558</v>
       </c>
       <c r="H812" t="s">
-        <v>2614</v>
+        <v>2616</v>
       </c>
       <c r="I812" t="s">
-        <v>2633</v>
+        <v>2635</v>
       </c>
       <c r="J812" t="s">
         <v>2647</v>
@@ -34310,7 +34310,7 @@
         <v>10</v>
       </c>
       <c r="B813" t="s">
-        <v>394</v>
+        <v>199</v>
       </c>
       <c r="C813" t="s">
         <v>1461</v>
@@ -34328,10 +34328,10 @@
         <v>2558</v>
       </c>
       <c r="H813" t="s">
-        <v>2615</v>
+        <v>2617</v>
       </c>
       <c r="I813" t="s">
-        <v>2634</v>
+        <v>2636</v>
       </c>
       <c r="J813" t="s">
         <v>2647</v>
@@ -34342,7 +34342,7 @@
         <v>10</v>
       </c>
       <c r="B814" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="C814" t="s">
         <v>1462</v>
@@ -34360,10 +34360,10 @@
         <v>2558</v>
       </c>
       <c r="H814" t="s">
-        <v>2616</v>
+        <v>2618</v>
       </c>
       <c r="I814" t="s">
-        <v>2635</v>
+        <v>2637</v>
       </c>
       <c r="J814" t="s">
         <v>2647</v>
@@ -34374,7 +34374,7 @@
         <v>10</v>
       </c>
       <c r="B815" t="s">
-        <v>199</v>
+        <v>386</v>
       </c>
       <c r="C815" t="s">
         <v>1463</v>
@@ -34392,10 +34392,10 @@
         <v>2558</v>
       </c>
       <c r="H815" t="s">
-        <v>2617</v>
+        <v>2619</v>
       </c>
       <c r="I815" t="s">
-        <v>2636</v>
+        <v>2638</v>
       </c>
       <c r="J815" t="s">
         <v>2647</v>
@@ -34406,7 +34406,7 @@
         <v>10</v>
       </c>
       <c r="B816" t="s">
-        <v>105</v>
+        <v>393</v>
       </c>
       <c r="C816" t="s">
         <v>1464</v>
@@ -34424,10 +34424,10 @@
         <v>2558</v>
       </c>
       <c r="H816" t="s">
-        <v>2618</v>
+        <v>2620</v>
       </c>
       <c r="I816" t="s">
-        <v>2637</v>
+        <v>2639</v>
       </c>
       <c r="J816" t="s">
         <v>2647</v>
@@ -34438,7 +34438,7 @@
         <v>10</v>
       </c>
       <c r="B817" t="s">
-        <v>388</v>
+        <v>22</v>
       </c>
       <c r="C817" t="s">
         <v>1465</v>
@@ -34456,10 +34456,10 @@
         <v>2558</v>
       </c>
       <c r="H817" t="s">
-        <v>2619</v>
+        <v>2621</v>
       </c>
       <c r="I817" t="s">
-        <v>2638</v>
+        <v>2640</v>
       </c>
       <c r="J817" t="s">
         <v>2647</v>
@@ -34470,7 +34470,7 @@
         <v>10</v>
       </c>
       <c r="B818" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C818" t="s">
         <v>1466</v>
@@ -34488,10 +34488,10 @@
         <v>2558</v>
       </c>
       <c r="H818" t="s">
-        <v>2620</v>
+        <v>2622</v>
       </c>
       <c r="I818" t="s">
-        <v>2639</v>
+        <v>2641</v>
       </c>
       <c r="J818" t="s">
         <v>2647</v>
@@ -34502,7 +34502,7 @@
         <v>10</v>
       </c>
       <c r="B819" t="s">
-        <v>22</v>
+        <v>313</v>
       </c>
       <c r="C819" t="s">
         <v>1467</v>
@@ -34520,10 +34520,10 @@
         <v>2558</v>
       </c>
       <c r="H819" t="s">
-        <v>2621</v>
+        <v>2623</v>
       </c>
       <c r="I819" t="s">
-        <v>2640</v>
+        <v>2642</v>
       </c>
       <c r="J819" t="s">
         <v>2647</v>
@@ -34534,7 +34534,7 @@
         <v>10</v>
       </c>
       <c r="B820" t="s">
-        <v>396</v>
+        <v>320</v>
       </c>
       <c r="C820" t="s">
         <v>1468</v>
@@ -34552,10 +34552,10 @@
         <v>2558</v>
       </c>
       <c r="H820" t="s">
-        <v>2622</v>
+        <v>2624</v>
       </c>
       <c r="I820" t="s">
-        <v>2641</v>
+        <v>2643</v>
       </c>
       <c r="J820" t="s">
         <v>2647</v>
@@ -34566,7 +34566,7 @@
         <v>10</v>
       </c>
       <c r="B821" t="s">
-        <v>313</v>
+        <v>18</v>
       </c>
       <c r="C821" t="s">
         <v>1469</v>
@@ -34584,10 +34584,10 @@
         <v>2558</v>
       </c>
       <c r="H821" t="s">
-        <v>2623</v>
+        <v>2625</v>
       </c>
       <c r="I821" t="s">
-        <v>2642</v>
+        <v>2644</v>
       </c>
       <c r="J821" t="s">
         <v>2647</v>
@@ -34598,7 +34598,7 @@
         <v>10</v>
       </c>
       <c r="B822" t="s">
-        <v>320</v>
+        <v>226</v>
       </c>
       <c r="C822" t="s">
         <v>1470</v>
@@ -34610,16 +34610,16 @@
         <v>2419</v>
       </c>
       <c r="F822" t="s">
-        <v>2471</v>
+        <v>2472</v>
       </c>
       <c r="G822" t="s">
-        <v>2558</v>
+        <v>2559</v>
       </c>
       <c r="H822" t="s">
-        <v>2624</v>
+        <v>2609</v>
       </c>
       <c r="I822" t="s">
-        <v>2643</v>
+        <v>2628</v>
       </c>
       <c r="J822" t="s">
         <v>2647</v>
@@ -34630,7 +34630,7 @@
         <v>10</v>
       </c>
       <c r="B823" t="s">
-        <v>18</v>
+        <v>201</v>
       </c>
       <c r="C823" t="s">
         <v>1471</v>
@@ -34642,16 +34642,16 @@
         <v>2419</v>
       </c>
       <c r="F823" t="s">
-        <v>2471</v>
+        <v>2472</v>
       </c>
       <c r="G823" t="s">
-        <v>2558</v>
+        <v>2559</v>
       </c>
       <c r="H823" t="s">
-        <v>2625</v>
+        <v>2610</v>
       </c>
       <c r="I823" t="s">
-        <v>2644</v>
+        <v>2629</v>
       </c>
       <c r="J823" t="s">
         <v>2647</v>
@@ -34662,7 +34662,7 @@
         <v>10</v>
       </c>
       <c r="B824" t="s">
-        <v>226</v>
+        <v>68</v>
       </c>
       <c r="C824" t="s">
         <v>1472</v>
@@ -34680,10 +34680,10 @@
         <v>2559</v>
       </c>
       <c r="H824" t="s">
-        <v>2609</v>
+        <v>2611</v>
       </c>
       <c r="I824" t="s">
-        <v>2628</v>
+        <v>2630</v>
       </c>
       <c r="J824" t="s">
         <v>2647</v>
@@ -34694,7 +34694,7 @@
         <v>10</v>
       </c>
       <c r="B825" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C825" t="s">
         <v>1473</v>
@@ -34712,10 +34712,10 @@
         <v>2559</v>
       </c>
       <c r="H825" t="s">
-        <v>2610</v>
+        <v>2612</v>
       </c>
       <c r="I825" t="s">
-        <v>2629</v>
+        <v>2631</v>
       </c>
       <c r="J825" t="s">
         <v>2647</v>
@@ -34726,7 +34726,7 @@
         <v>10</v>
       </c>
       <c r="B826" t="s">
-        <v>68</v>
+        <v>395</v>
       </c>
       <c r="C826" t="s">
         <v>1474</v>
@@ -34744,10 +34744,10 @@
         <v>2559</v>
       </c>
       <c r="H826" t="s">
-        <v>2611</v>
+        <v>2613</v>
       </c>
       <c r="I826" t="s">
-        <v>2630</v>
+        <v>2632</v>
       </c>
       <c r="J826" t="s">
         <v>2647</v>
@@ -34758,7 +34758,7 @@
         <v>10</v>
       </c>
       <c r="B827" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="C827" t="s">
         <v>1475</v>
@@ -34776,10 +34776,10 @@
         <v>2559</v>
       </c>
       <c r="H827" t="s">
-        <v>2612</v>
+        <v>2614</v>
       </c>
       <c r="I827" t="s">
-        <v>2631</v>
+        <v>2633</v>
       </c>
       <c r="J827" t="s">
         <v>2647</v>
@@ -34790,7 +34790,7 @@
         <v>10</v>
       </c>
       <c r="B828" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C828" t="s">
         <v>1476</v>
@@ -34808,10 +34808,10 @@
         <v>2559</v>
       </c>
       <c r="H828" t="s">
-        <v>2613</v>
+        <v>2615</v>
       </c>
       <c r="I828" t="s">
-        <v>2632</v>
+        <v>2634</v>
       </c>
       <c r="J828" t="s">
         <v>2647</v>
@@ -34822,7 +34822,7 @@
         <v>10</v>
       </c>
       <c r="B829" t="s">
-        <v>192</v>
+        <v>52</v>
       </c>
       <c r="C829" t="s">
         <v>1477</v>
@@ -34840,10 +34840,10 @@
         <v>2559</v>
       </c>
       <c r="H829" t="s">
-        <v>2614</v>
+        <v>2616</v>
       </c>
       <c r="I829" t="s">
-        <v>2633</v>
+        <v>2635</v>
       </c>
       <c r="J829" t="s">
         <v>2647</v>
@@ -34854,7 +34854,7 @@
         <v>10</v>
       </c>
       <c r="B830" t="s">
-        <v>398</v>
+        <v>40</v>
       </c>
       <c r="C830" t="s">
         <v>1478</v>
@@ -34872,10 +34872,10 @@
         <v>2559</v>
       </c>
       <c r="H830" t="s">
-        <v>2615</v>
+        <v>2617</v>
       </c>
       <c r="I830" t="s">
-        <v>2634</v>
+        <v>2636</v>
       </c>
       <c r="J830" t="s">
         <v>2647</v>
@@ -34886,7 +34886,7 @@
         <v>10</v>
       </c>
       <c r="B831" t="s">
-        <v>52</v>
+        <v>317</v>
       </c>
       <c r="C831" t="s">
         <v>1479</v>
@@ -34904,10 +34904,10 @@
         <v>2559</v>
       </c>
       <c r="H831" t="s">
-        <v>2616</v>
+        <v>2618</v>
       </c>
       <c r="I831" t="s">
-        <v>2635</v>
+        <v>2637</v>
       </c>
       <c r="J831" t="s">
         <v>2647</v>
@@ -34918,7 +34918,7 @@
         <v>10</v>
       </c>
       <c r="B832" t="s">
-        <v>40</v>
+        <v>397</v>
       </c>
       <c r="C832" t="s">
         <v>1480</v>
@@ -34936,10 +34936,10 @@
         <v>2559</v>
       </c>
       <c r="H832" t="s">
-        <v>2617</v>
+        <v>2619</v>
       </c>
       <c r="I832" t="s">
-        <v>2636</v>
+        <v>2638</v>
       </c>
       <c r="J832" t="s">
         <v>2647</v>
@@ -34950,7 +34950,7 @@
         <v>10</v>
       </c>
       <c r="B833" t="s">
-        <v>317</v>
+        <v>232</v>
       </c>
       <c r="C833" t="s">
         <v>1481</v>
@@ -34968,10 +34968,10 @@
         <v>2559</v>
       </c>
       <c r="H833" t="s">
-        <v>2618</v>
+        <v>2620</v>
       </c>
       <c r="I833" t="s">
-        <v>2637</v>
+        <v>2639</v>
       </c>
       <c r="J833" t="s">
         <v>2647</v>
@@ -34982,7 +34982,7 @@
         <v>10</v>
       </c>
       <c r="B834" t="s">
-        <v>399</v>
+        <v>54</v>
       </c>
       <c r="C834" t="s">
         <v>1482</v>
@@ -35000,10 +35000,10 @@
         <v>2559</v>
       </c>
       <c r="H834" t="s">
-        <v>2619</v>
+        <v>2621</v>
       </c>
       <c r="I834" t="s">
-        <v>2638</v>
+        <v>2640</v>
       </c>
       <c r="J834" t="s">
         <v>2647</v>
@@ -35014,7 +35014,7 @@
         <v>10</v>
       </c>
       <c r="B835" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="C835" t="s">
         <v>1483</v>
@@ -35032,10 +35032,10 @@
         <v>2559</v>
       </c>
       <c r="H835" t="s">
-        <v>2620</v>
+        <v>2622</v>
       </c>
       <c r="I835" t="s">
-        <v>2639</v>
+        <v>2641</v>
       </c>
       <c r="J835" t="s">
         <v>2647</v>
@@ -35046,7 +35046,7 @@
         <v>10</v>
       </c>
       <c r="B836" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="C836" t="s">
         <v>1484</v>
@@ -35064,10 +35064,10 @@
         <v>2559</v>
       </c>
       <c r="H836" t="s">
-        <v>2621</v>
+        <v>2623</v>
       </c>
       <c r="I836" t="s">
-        <v>2640</v>
+        <v>2642</v>
       </c>
       <c r="J836" t="s">
         <v>2647</v>
@@ -35078,7 +35078,7 @@
         <v>10</v>
       </c>
       <c r="B837" t="s">
-        <v>214</v>
+        <v>111</v>
       </c>
       <c r="C837" t="s">
         <v>1485</v>
@@ -35096,10 +35096,10 @@
         <v>2559</v>
       </c>
       <c r="H837" t="s">
-        <v>2622</v>
+        <v>2624</v>
       </c>
       <c r="I837" t="s">
-        <v>2641</v>
+        <v>2643</v>
       </c>
       <c r="J837" t="s">
         <v>2647</v>
@@ -35110,7 +35110,7 @@
         <v>10</v>
       </c>
       <c r="B838" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C838" t="s">
         <v>1486</v>
@@ -35128,10 +35128,10 @@
         <v>2559</v>
       </c>
       <c r="H838" t="s">
-        <v>2623</v>
+        <v>2625</v>
       </c>
       <c r="I838" t="s">
-        <v>2642</v>
+        <v>2644</v>
       </c>
       <c r="J838" t="s">
         <v>2647</v>
@@ -35142,28 +35142,28 @@
         <v>10</v>
       </c>
       <c r="B839" t="s">
-        <v>111</v>
+        <v>398</v>
       </c>
       <c r="C839" t="s">
         <v>1487</v>
       </c>
       <c r="D839" t="s">
-        <v>2401</v>
+        <v>2402</v>
       </c>
       <c r="E839" t="s">
-        <v>2419</v>
+        <v>2420</v>
       </c>
       <c r="F839" t="s">
-        <v>2472</v>
+        <v>2473</v>
       </c>
       <c r="G839" t="s">
-        <v>2559</v>
+        <v>2420</v>
       </c>
       <c r="H839" t="s">
-        <v>2624</v>
+        <v>2609</v>
       </c>
       <c r="I839" t="s">
-        <v>2643</v>
+        <v>2628</v>
       </c>
       <c r="J839" t="s">
         <v>2647</v>
@@ -35174,28 +35174,28 @@
         <v>10</v>
       </c>
       <c r="B840" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="C840" t="s">
         <v>1488</v>
       </c>
       <c r="D840" t="s">
-        <v>2401</v>
+        <v>2402</v>
       </c>
       <c r="E840" t="s">
-        <v>2419</v>
+        <v>2420</v>
       </c>
       <c r="F840" t="s">
-        <v>2472</v>
+        <v>2473</v>
       </c>
       <c r="G840" t="s">
-        <v>2559</v>
+        <v>2420</v>
       </c>
       <c r="H840" t="s">
-        <v>2625</v>
+        <v>2626</v>
       </c>
       <c r="I840" t="s">
-        <v>2644</v>
+        <v>2645</v>
       </c>
       <c r="J840" t="s">
         <v>2647</v>
@@ -35206,7 +35206,7 @@
         <v>10</v>
       </c>
       <c r="B841" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C841" t="s">
         <v>1489</v>
@@ -35224,10 +35224,10 @@
         <v>2420</v>
       </c>
       <c r="H841" t="s">
-        <v>2609</v>
+        <v>2610</v>
       </c>
       <c r="I841" t="s">
-        <v>2628</v>
+        <v>2629</v>
       </c>
       <c r="J841" t="s">
         <v>2647</v>
@@ -35238,7 +35238,7 @@
         <v>10</v>
       </c>
       <c r="B842" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="C842" t="s">
         <v>1490</v>
@@ -35256,10 +35256,10 @@
         <v>2420</v>
       </c>
       <c r="H842" t="s">
-        <v>2626</v>
+        <v>2627</v>
       </c>
       <c r="I842" t="s">
-        <v>2645</v>
+        <v>2646</v>
       </c>
       <c r="J842" t="s">
         <v>2647</v>
@@ -35270,7 +35270,7 @@
         <v>10</v>
       </c>
       <c r="B843" t="s">
-        <v>401</v>
+        <v>36</v>
       </c>
       <c r="C843" t="s">
         <v>1491</v>
@@ -35288,10 +35288,10 @@
         <v>2420</v>
       </c>
       <c r="H843" t="s">
-        <v>2610</v>
+        <v>2611</v>
       </c>
       <c r="I843" t="s">
-        <v>2629</v>
+        <v>2630</v>
       </c>
       <c r="J843" t="s">
         <v>2647</v>
@@ -35302,7 +35302,7 @@
         <v>10</v>
       </c>
       <c r="B844" t="s">
-        <v>86</v>
+        <v>400</v>
       </c>
       <c r="C844" t="s">
         <v>1492</v>
@@ -35320,10 +35320,10 @@
         <v>2420</v>
       </c>
       <c r="H844" t="s">
-        <v>2627</v>
+        <v>2612</v>
       </c>
       <c r="I844" t="s">
-        <v>2646</v>
+        <v>2631</v>
       </c>
       <c r="J844" t="s">
         <v>2647</v>
@@ -35334,7 +35334,7 @@
         <v>10</v>
       </c>
       <c r="B845" t="s">
-        <v>36</v>
+        <v>401</v>
       </c>
       <c r="C845" t="s">
         <v>1493</v>
@@ -35352,10 +35352,10 @@
         <v>2420</v>
       </c>
       <c r="H845" t="s">
-        <v>2611</v>
+        <v>2613</v>
       </c>
       <c r="I845" t="s">
-        <v>2630</v>
+        <v>2632</v>
       </c>
       <c r="J845" t="s">
         <v>2647</v>
@@ -35366,7 +35366,7 @@
         <v>10</v>
       </c>
       <c r="B846" t="s">
-        <v>402</v>
+        <v>121</v>
       </c>
       <c r="C846" t="s">
         <v>1494</v>
@@ -35384,10 +35384,10 @@
         <v>2420</v>
       </c>
       <c r="H846" t="s">
-        <v>2612</v>
+        <v>2614</v>
       </c>
       <c r="I846" t="s">
-        <v>2631</v>
+        <v>2633</v>
       </c>
       <c r="J846" t="s">
         <v>2647</v>
@@ -35398,7 +35398,7 @@
         <v>10</v>
       </c>
       <c r="B847" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C847" t="s">
         <v>1495</v>
@@ -35416,10 +35416,10 @@
         <v>2420</v>
       </c>
       <c r="H847" t="s">
-        <v>2613</v>
+        <v>2615</v>
       </c>
       <c r="I847" t="s">
-        <v>2632</v>
+        <v>2634</v>
       </c>
       <c r="J847" t="s">
         <v>2647</v>
@@ -35430,7 +35430,7 @@
         <v>10</v>
       </c>
       <c r="B848" t="s">
-        <v>121</v>
+        <v>317</v>
       </c>
       <c r="C848" t="s">
         <v>1496</v>
@@ -35448,10 +35448,10 @@
         <v>2420</v>
       </c>
       <c r="H848" t="s">
-        <v>2614</v>
+        <v>2616</v>
       </c>
       <c r="I848" t="s">
-        <v>2633</v>
+        <v>2635</v>
       </c>
       <c r="J848" t="s">
         <v>2647</v>
@@ -35462,7 +35462,7 @@
         <v>10</v>
       </c>
       <c r="B849" t="s">
-        <v>404</v>
+        <v>93</v>
       </c>
       <c r="C849" t="s">
         <v>1497</v>
@@ -35480,10 +35480,10 @@
         <v>2420</v>
       </c>
       <c r="H849" t="s">
-        <v>2615</v>
+        <v>2617</v>
       </c>
       <c r="I849" t="s">
-        <v>2634</v>
+        <v>2636</v>
       </c>
       <c r="J849" t="s">
         <v>2647</v>
@@ -35494,7 +35494,7 @@
         <v>10</v>
       </c>
       <c r="B850" t="s">
-        <v>317</v>
+        <v>198</v>
       </c>
       <c r="C850" t="s">
         <v>1498</v>
@@ -35512,10 +35512,10 @@
         <v>2420</v>
       </c>
       <c r="H850" t="s">
-        <v>2616</v>
+        <v>2618</v>
       </c>
       <c r="I850" t="s">
-        <v>2635</v>
+        <v>2637</v>
       </c>
       <c r="J850" t="s">
         <v>2647</v>
@@ -35526,7 +35526,7 @@
         <v>10</v>
       </c>
       <c r="B851" t="s">
-        <v>93</v>
+        <v>403</v>
       </c>
       <c r="C851" t="s">
         <v>1499</v>
@@ -35544,10 +35544,10 @@
         <v>2420</v>
       </c>
       <c r="H851" t="s">
-        <v>2617</v>
+        <v>2619</v>
       </c>
       <c r="I851" t="s">
-        <v>2636</v>
+        <v>2638</v>
       </c>
       <c r="J851" t="s">
         <v>2647</v>
@@ -35558,7 +35558,7 @@
         <v>10</v>
       </c>
       <c r="B852" t="s">
-        <v>198</v>
+        <v>404</v>
       </c>
       <c r="C852" t="s">
         <v>1500</v>
@@ -35576,10 +35576,10 @@
         <v>2420</v>
       </c>
       <c r="H852" t="s">
-        <v>2618</v>
+        <v>2620</v>
       </c>
       <c r="I852" t="s">
-        <v>2637</v>
+        <v>2639</v>
       </c>
       <c r="J852" t="s">
         <v>2647</v>
@@ -35590,7 +35590,7 @@
         <v>10</v>
       </c>
       <c r="B853" t="s">
-        <v>405</v>
+        <v>105</v>
       </c>
       <c r="C853" t="s">
         <v>1501</v>
@@ -35608,10 +35608,10 @@
         <v>2420</v>
       </c>
       <c r="H853" t="s">
-        <v>2619</v>
+        <v>2621</v>
       </c>
       <c r="I853" t="s">
-        <v>2638</v>
+        <v>2640</v>
       </c>
       <c r="J853" t="s">
         <v>2647</v>
@@ -35622,7 +35622,7 @@
         <v>10</v>
       </c>
       <c r="B854" t="s">
-        <v>406</v>
+        <v>332</v>
       </c>
       <c r="C854" t="s">
         <v>1502</v>
@@ -35640,10 +35640,10 @@
         <v>2420</v>
       </c>
       <c r="H854" t="s">
-        <v>2620</v>
+        <v>2622</v>
       </c>
       <c r="I854" t="s">
-        <v>2639</v>
+        <v>2641</v>
       </c>
       <c r="J854" t="s">
         <v>2647</v>
@@ -35654,7 +35654,7 @@
         <v>10</v>
       </c>
       <c r="B855" t="s">
-        <v>105</v>
+        <v>216</v>
       </c>
       <c r="C855" t="s">
         <v>1503</v>
@@ -35672,10 +35672,10 @@
         <v>2420</v>
       </c>
       <c r="H855" t="s">
-        <v>2621</v>
+        <v>2623</v>
       </c>
       <c r="I855" t="s">
-        <v>2640</v>
+        <v>2642</v>
       </c>
       <c r="J855" t="s">
         <v>2647</v>
@@ -35686,7 +35686,7 @@
         <v>10</v>
       </c>
       <c r="B856" t="s">
-        <v>332</v>
+        <v>191</v>
       </c>
       <c r="C856" t="s">
         <v>1504</v>
@@ -35704,10 +35704,10 @@
         <v>2420</v>
       </c>
       <c r="H856" t="s">
-        <v>2622</v>
+        <v>2624</v>
       </c>
       <c r="I856" t="s">
-        <v>2641</v>
+        <v>2643</v>
       </c>
       <c r="J856" t="s">
         <v>2647</v>
@@ -35718,7 +35718,7 @@
         <v>10</v>
       </c>
       <c r="B857" t="s">
-        <v>216</v>
+        <v>68</v>
       </c>
       <c r="C857" t="s">
         <v>1505</v>
@@ -35736,10 +35736,10 @@
         <v>2420</v>
       </c>
       <c r="H857" t="s">
-        <v>2623</v>
+        <v>2625</v>
       </c>
       <c r="I857" t="s">
-        <v>2642</v>
+        <v>2644</v>
       </c>
       <c r="J857" t="s">
         <v>2647</v>
@@ -35750,28 +35750,28 @@
         <v>10</v>
       </c>
       <c r="B858" t="s">
-        <v>191</v>
+        <v>40</v>
       </c>
       <c r="C858" t="s">
         <v>1506</v>
       </c>
       <c r="D858" t="s">
-        <v>2402</v>
+        <v>2403</v>
       </c>
       <c r="E858" t="s">
-        <v>2420</v>
+        <v>2421</v>
       </c>
       <c r="F858" t="s">
-        <v>2473</v>
+        <v>2474</v>
       </c>
       <c r="G858" t="s">
-        <v>2420</v>
+        <v>2421</v>
       </c>
       <c r="H858" t="s">
-        <v>2624</v>
+        <v>2609</v>
       </c>
       <c r="I858" t="s">
-        <v>2643</v>
+        <v>2628</v>
       </c>
       <c r="J858" t="s">
         <v>2647</v>
@@ -35782,28 +35782,28 @@
         <v>10</v>
       </c>
       <c r="B859" t="s">
-        <v>68</v>
+        <v>405</v>
       </c>
       <c r="C859" t="s">
         <v>1507</v>
       </c>
       <c r="D859" t="s">
-        <v>2402</v>
+        <v>2403</v>
       </c>
       <c r="E859" t="s">
-        <v>2420</v>
+        <v>2421</v>
       </c>
       <c r="F859" t="s">
-        <v>2473</v>
+        <v>2474</v>
       </c>
       <c r="G859" t="s">
-        <v>2420</v>
+        <v>2421</v>
       </c>
       <c r="H859" t="s">
-        <v>2625</v>
+        <v>2610</v>
       </c>
       <c r="I859" t="s">
-        <v>2644</v>
+        <v>2629</v>
       </c>
       <c r="J859" t="s">
         <v>2647</v>
@@ -35814,7 +35814,7 @@
         <v>10</v>
       </c>
       <c r="B860" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="C860" t="s">
         <v>1508</v>
@@ -35832,10 +35832,10 @@
         <v>2421</v>
       </c>
       <c r="H860" t="s">
-        <v>2609</v>
+        <v>2627</v>
       </c>
       <c r="I860" t="s">
-        <v>2628</v>
+        <v>2646</v>
       </c>
       <c r="J860" t="s">
         <v>2647</v>
@@ -35846,7 +35846,7 @@
         <v>10</v>
       </c>
       <c r="B861" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="C861" t="s">
         <v>1509</v>
@@ -35864,10 +35864,10 @@
         <v>2421</v>
       </c>
       <c r="H861" t="s">
-        <v>2626</v>
+        <v>2611</v>
       </c>
       <c r="I861" t="s">
-        <v>2645</v>
+        <v>2630</v>
       </c>
       <c r="J861" t="s">
         <v>2647</v>
@@ -35878,7 +35878,7 @@
         <v>10</v>
       </c>
       <c r="B862" t="s">
-        <v>240</v>
+        <v>24</v>
       </c>
       <c r="C862" t="s">
         <v>1510</v>
@@ -35896,10 +35896,10 @@
         <v>2421</v>
       </c>
       <c r="H862" t="s">
-        <v>2610</v>
+        <v>2612</v>
       </c>
       <c r="I862" t="s">
-        <v>2629</v>
+        <v>2631</v>
       </c>
       <c r="J862" t="s">
         <v>2647</v>
@@ -35910,7 +35910,7 @@
         <v>10</v>
       </c>
       <c r="B863" t="s">
-        <v>232</v>
+        <v>158</v>
       </c>
       <c r="C863" t="s">
         <v>1511</v>
@@ -35928,10 +35928,10 @@
         <v>2421</v>
       </c>
       <c r="H863" t="s">
-        <v>2612</v>
+        <v>2613</v>
       </c>
       <c r="I863" t="s">
-        <v>2631</v>
+        <v>2632</v>
       </c>
       <c r="J863" t="s">
         <v>2647</v>
@@ -35942,7 +35942,7 @@
         <v>10</v>
       </c>
       <c r="B864" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C864" t="s">
         <v>1512</v>
@@ -35960,10 +35960,10 @@
         <v>2421</v>
       </c>
       <c r="H864" t="s">
-        <v>2613</v>
+        <v>2614</v>
       </c>
       <c r="I864" t="s">
-        <v>2632</v>
+        <v>2633</v>
       </c>
       <c r="J864" t="s">
         <v>2647</v>
@@ -35974,7 +35974,7 @@
         <v>10</v>
       </c>
       <c r="B865" t="s">
-        <v>95</v>
+        <v>382</v>
       </c>
       <c r="C865" t="s">
         <v>1513</v>
@@ -35992,10 +35992,10 @@
         <v>2421</v>
       </c>
       <c r="H865" t="s">
-        <v>2614</v>
+        <v>2615</v>
       </c>
       <c r="I865" t="s">
-        <v>2633</v>
+        <v>2634</v>
       </c>
       <c r="J865" t="s">
         <v>2647</v>
@@ -36006,7 +36006,7 @@
         <v>10</v>
       </c>
       <c r="B866" t="s">
-        <v>112</v>
+        <v>346</v>
       </c>
       <c r="C866" t="s">
         <v>1514</v>
@@ -36024,10 +36024,10 @@
         <v>2421</v>
       </c>
       <c r="H866" t="s">
-        <v>2615</v>
+        <v>2616</v>
       </c>
       <c r="I866" t="s">
-        <v>2634</v>
+        <v>2635</v>
       </c>
       <c r="J866" t="s">
         <v>2647</v>
@@ -36038,7 +36038,7 @@
         <v>10</v>
       </c>
       <c r="B867" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="C867" t="s">
         <v>1515</v>
@@ -36056,10 +36056,10 @@
         <v>2421</v>
       </c>
       <c r="H867" t="s">
-        <v>2616</v>
+        <v>2617</v>
       </c>
       <c r="I867" t="s">
-        <v>2635</v>
+        <v>2636</v>
       </c>
       <c r="J867" t="s">
         <v>2647</v>
@@ -36070,7 +36070,7 @@
         <v>10</v>
       </c>
       <c r="B868" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="C868" t="s">
         <v>1516</v>
@@ -36088,10 +36088,10 @@
         <v>2421</v>
       </c>
       <c r="H868" t="s">
-        <v>2617</v>
+        <v>2618</v>
       </c>
       <c r="I868" t="s">
-        <v>2636</v>
+        <v>2637</v>
       </c>
       <c r="J868" t="s">
         <v>2647</v>
@@ -36102,7 +36102,7 @@
         <v>10</v>
       </c>
       <c r="B869" t="s">
-        <v>62</v>
+        <v>407</v>
       </c>
       <c r="C869" t="s">
         <v>1517</v>
@@ -36120,10 +36120,10 @@
         <v>2421</v>
       </c>
       <c r="H869" t="s">
-        <v>2618</v>
+        <v>2619</v>
       </c>
       <c r="I869" t="s">
-        <v>2637</v>
+        <v>2638</v>
       </c>
       <c r="J869" t="s">
         <v>2647</v>
@@ -36134,7 +36134,7 @@
         <v>10</v>
       </c>
       <c r="B870" t="s">
-        <v>76</v>
+        <v>326</v>
       </c>
       <c r="C870" t="s">
         <v>1518</v>
@@ -36152,10 +36152,10 @@
         <v>2421</v>
       </c>
       <c r="H870" t="s">
-        <v>2619</v>
+        <v>2620</v>
       </c>
       <c r="I870" t="s">
-        <v>2638</v>
+        <v>2639</v>
       </c>
       <c r="J870" t="s">
         <v>2647</v>
@@ -36166,7 +36166,7 @@
         <v>10</v>
       </c>
       <c r="B871" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="C871" t="s">
         <v>1519</v>
@@ -36184,10 +36184,10 @@
         <v>2421</v>
       </c>
       <c r="H871" t="s">
-        <v>2620</v>
+        <v>2621</v>
       </c>
       <c r="I871" t="s">
-        <v>2639</v>
+        <v>2640</v>
       </c>
       <c r="J871" t="s">
         <v>2647</v>
@@ -36198,7 +36198,7 @@
         <v>10</v>
       </c>
       <c r="B872" t="s">
-        <v>27</v>
+        <v>352</v>
       </c>
       <c r="C872" t="s">
         <v>1520</v>
@@ -36216,10 +36216,10 @@
         <v>2421</v>
       </c>
       <c r="H872" t="s">
-        <v>2621</v>
+        <v>2622</v>
       </c>
       <c r="I872" t="s">
-        <v>2640</v>
+        <v>2641</v>
       </c>
       <c r="J872" t="s">
         <v>2647</v>
@@ -36230,7 +36230,7 @@
         <v>10</v>
       </c>
       <c r="B873" t="s">
-        <v>169</v>
+        <v>363</v>
       </c>
       <c r="C873" t="s">
         <v>1521</v>
@@ -36248,10 +36248,10 @@
         <v>2421</v>
       </c>
       <c r="H873" t="s">
-        <v>2622</v>
+        <v>2623</v>
       </c>
       <c r="I873" t="s">
-        <v>2641</v>
+        <v>2642</v>
       </c>
       <c r="J873" t="s">
         <v>2647</v>
@@ -36262,7 +36262,7 @@
         <v>10</v>
       </c>
       <c r="B874" t="s">
-        <v>13</v>
+        <v>406</v>
       </c>
       <c r="C874" t="s">
         <v>1522</v>
@@ -36280,10 +36280,10 @@
         <v>2421</v>
       </c>
       <c r="H874" t="s">
-        <v>2623</v>
+        <v>2624</v>
       </c>
       <c r="I874" t="s">
-        <v>2642</v>
+        <v>2643</v>
       </c>
       <c r="J874" t="s">
         <v>2647</v>
@@ -36294,7 +36294,7 @@
         <v>10</v>
       </c>
       <c r="B875" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C875" t="s">
         <v>1523</v>
@@ -36312,10 +36312,10 @@
         <v>2421</v>
       </c>
       <c r="H875" t="s">
-        <v>2624</v>
+        <v>2625</v>
       </c>
       <c r="I875" t="s">
-        <v>2643</v>
+        <v>2644</v>
       </c>
       <c r="J875" t="s">
         <v>2647</v>
@@ -37286,7 +37286,7 @@
         <v>10</v>
       </c>
       <c r="B906" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C906" t="s">
         <v>1554</v>
@@ -38662,7 +38662,7 @@
         <v>10</v>
       </c>
       <c r="B949" t="s">
-        <v>373</v>
+        <v>407</v>
       </c>
       <c r="C949" t="s">
         <v>1597</v>
@@ -39014,7 +39014,7 @@
         <v>10</v>
       </c>
       <c r="B960" t="s">
-        <v>371</v>
+        <v>406</v>
       </c>
       <c r="C960" t="s">
         <v>1608</v>
@@ -42086,7 +42086,7 @@
         <v>10</v>
       </c>
       <c r="B1056" t="s">
-        <v>371</v>
+        <v>406</v>
       </c>
       <c r="C1056" t="s">
         <v>1704</v>
@@ -43462,7 +43462,7 @@
         <v>10</v>
       </c>
       <c r="B1099" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C1099" t="s">
         <v>1747</v>
@@ -43910,7 +43910,7 @@
         <v>10</v>
       </c>
       <c r="B1113" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C1113" t="s">
         <v>1761</v>
@@ -45702,7 +45702,7 @@
         <v>10</v>
       </c>
       <c r="B1169" t="s">
-        <v>370</v>
+        <v>405</v>
       </c>
       <c r="C1169" t="s">
         <v>1817</v>
@@ -47206,7 +47206,7 @@
         <v>10</v>
       </c>
       <c r="B1216" t="s">
-        <v>373</v>
+        <v>407</v>
       </c>
       <c r="C1216" t="s">
         <v>1864</v>
@@ -47238,7 +47238,7 @@
         <v>10</v>
       </c>
       <c r="B1217" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C1217" t="s">
         <v>1865</v>
@@ -48294,7 +48294,7 @@
         <v>10</v>
       </c>
       <c r="B1250" t="s">
-        <v>407</v>
+        <v>370</v>
       </c>
       <c r="C1250" t="s">
         <v>1897</v>
@@ -48518,7 +48518,7 @@
         <v>10</v>
       </c>
       <c r="B1257" t="s">
-        <v>371</v>
+        <v>406</v>
       </c>
       <c r="C1257" t="s">
         <v>1904</v>
@@ -51398,7 +51398,7 @@
         <v>10</v>
       </c>
       <c r="B1347" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C1347" t="s">
         <v>1994</v>
@@ -53414,7 +53414,7 @@
         <v>10</v>
       </c>
       <c r="B1410" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C1410" t="s">
         <v>2057</v>
@@ -53542,7 +53542,7 @@
         <v>10</v>
       </c>
       <c r="B1414" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C1414" t="s">
         <v>2061</v>
@@ -54278,7 +54278,7 @@
         <v>10</v>
       </c>
       <c r="B1437" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C1437" t="s">
         <v>2084</v>
@@ -55046,7 +55046,7 @@
         <v>10</v>
       </c>
       <c r="B1461" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C1461" t="s">
         <v>2108</v>
@@ -56198,7 +56198,7 @@
         <v>10</v>
       </c>
       <c r="B1497" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C1497" t="s">
         <v>2144</v>
@@ -58790,7 +58790,7 @@
         <v>10</v>
       </c>
       <c r="B1578" t="s">
-        <v>407</v>
+        <v>370</v>
       </c>
       <c r="C1578" t="s">
         <v>2225</v>
@@ -60646,7 +60646,7 @@
         <v>10</v>
       </c>
       <c r="B1636" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="C1636" t="s">
         <v>2283</v>
@@ -61510,7 +61510,7 @@
         <v>10</v>
       </c>
       <c r="B1663" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C1663" t="s">
         <v>2309</v>
@@ -61574,7 +61574,7 @@
         <v>10</v>
       </c>
       <c r="B1665" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C1665" t="s">
         <v>2311</v>
@@ -63910,7 +63910,7 @@
         <v>10</v>
       </c>
       <c r="B1738" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C1738" t="s">
         <v>2384</v>

</xml_diff>